<commit_message>
update & lock sheet
</commit_message>
<xml_diff>
--- a/Dashboard.xlsx
+++ b/Dashboard.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vijay Purohit\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vijay Purohit\Desktop\M.Tech  (Data Science)\Masters Peojects  - Github\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="20460" windowHeight="9000" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="20415" windowHeight="7710" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MetaData" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4624" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4618" uniqueCount="556">
   <si>
     <t>Data Dictionary</t>
   </si>
@@ -1782,7 +1782,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1869,38 +1869,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1930,13 +1904,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5676,16 +5647,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>296617</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>222534</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>154565</xdr:rowOff>
+      <xdr:rowOff>59315</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>136121</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>154565</xdr:rowOff>
+      <xdr:colOff>624417</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>10584</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5712,16 +5683,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>272890</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>505725</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:colOff>645584</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>17993</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5749,15 +5720,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>589987</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>187295</xdr:rowOff>
+      <xdr:colOff>335985</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>287568</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>187295</xdr:rowOff>
+      <xdr:colOff>52916</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5785,15 +5756,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>597694</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>74771</xdr:rowOff>
+      <xdr:colOff>354278</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158749</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>44291</xdr:rowOff>
+      <xdr:colOff>21166</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>179917</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -27314,8 +27285,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A32:E39" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A18:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
       <items count="8">
@@ -27329,13 +27300,59 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="6">
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Salary" fld="1" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A5:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
+        <item x="4"/>
         <item x="2"/>
-        <item x="3"/>
-        <item h="1" x="4"/>
+        <item h="1" x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -27363,112 +27380,11 @@
       <x v="5"/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of PerformanceScore" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="H32:N39" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item h="1" x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="8">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of RaceDesc" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of Department" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -27480,75 +27396,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D5:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisCol" dataField="1" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item h="1" x="1"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="1">
-    <i>
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of EmploymentStatus" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="H20:I27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="36">
@@ -27680,7 +27527,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D18:F25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
@@ -27751,118 +27598,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A18:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item h="1" x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Salary" fld="1" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A5:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item h="1" x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Department" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H1:L9" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
@@ -28069,6 +27805,241 @@
   <dataFields count="2">
     <dataField name="Average of EngagementSurvey" fld="2" subtotal="average" baseField="1" baseItem="2" numFmtId="164"/>
     <dataField name="Average of EmpSatisfaction" fld="3" subtotal="average" baseField="1" baseItem="2" numFmtId="164"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A32:E39" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item h="1" x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item h="1" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of PerformanceScore" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D5:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisCol" dataField="1" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item h="1" x="1"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="1">
+    <i>
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of EmploymentStatus" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H32:N39" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item h="1" x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="8">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of RaceDesc" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -28794,8 +28765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS314"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="AA1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63856,6 +63827,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="qwwKWpaRYrFuEaZXwYRv9WLMNw2eYTzb6Hdk8n+gQlNH4GxZG9Z37DZczPgGD7GiQ/70tL5z+BXMJOErA7EytQ==" saltValue="uRVAFMeT6XAWQtqHom732g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -63863,10 +63835,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X48"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="J26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+    <sheetView topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64383,7 +64355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>541</v>
       </c>
@@ -64428,7 +64400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>173</v>
       </c>
@@ -64459,7 +64431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>349</v>
       </c>
@@ -64488,7 +64460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>102</v>
       </c>
@@ -64527,7 +64499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>93</v>
       </c>
@@ -64572,7 +64544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>188</v>
       </c>
@@ -64608,7 +64580,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>122</v>
       </c>
@@ -64637,52 +64609,8 @@
       <c r="N39" s="6">
         <v>5</v>
       </c>
-      <c r="S39" s="25" t="s">
-        <v>392</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>305</v>
-      </c>
-      <c r="U39" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="V39" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="W39" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="X39" s="25" t="s">
-        <v>90</v>
-      </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="S40" s="24">
-        <f>VLOOKUP(Dashboard!$U$6,$H$34:$N$39,5,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="T40" s="26">
-        <f>VLOOKUP(Dashboard!$U$6,$H$34:$N$39,2,TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="U40" s="24">
-        <f>VLOOKUP(Dashboard!$U$6,$H$34:$N$39,3,TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="V40" s="26">
-        <f>VLOOKUP(Dashboard!$U$6,$H$34:$N$39,6,TRUE)</f>
-        <v>5</v>
-      </c>
-      <c r="W40" s="24">
-        <f>VLOOKUP(Dashboard!$U$6,$H$34:$N$39,4,TRUE)</f>
-        <v>10</v>
-      </c>
-      <c r="X40" s="26">
-        <f>VLOOKUP(Dashboard!$U$6,$H$34:$N$39,7,TRUE)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
         <v>96</v>
       </c>
@@ -64713,9 +64641,9 @@
       <c r="N42" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="P42" s="27"/>
+      <c r="P42" s="23"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B43">
         <f>VLOOKUP(Dashboard!U6,Pivot_Tables!A34:E39,2,TRUE)</f>
         <v>2</v>
@@ -64756,24 +64684,25 @@
         <f>VLOOKUP(Dashboard!U6,H33:N39,7,TRUE)</f>
         <v>14</v>
       </c>
-      <c r="P43" s="27"/>
+      <c r="P43" s="23"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="P44" s="27"/>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P44" s="23"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="P45" s="27"/>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P45" s="23"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="P46" s="27"/>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P46" s="23"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="P47" s="27"/>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P47" s="23"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P48" s="5"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="BJztoS/9/Dy/ihklSnvXUQRDJt3UwrcoQPWhoWRQYAHkIMbYtcvk12p5YJWN5fsbxvyT20Up8ML7wJUNCGu6yQ==" saltValue="buZrCsw7aSbPD+PM4HyeRg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId9"/>
@@ -64784,10 +64713,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6:W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64799,167 +64728,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>535</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U6" s="30" t="s">
+      <c r="U6" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
+      <c r="G7" s="21" t="s">
+        <v>536</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>537</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>538</v>
+      </c>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
     </row>
     <row r="8" spans="1:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G8" s="21" t="s">
-        <v>536</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>537</v>
-      </c>
-      <c r="K8" s="21" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="G9" s="22">
+      <c r="G8" s="22">
         <f>VLOOKUP(U6,Pivot_Tables!A6:B11,2,FALSE)</f>
         <v>31</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I8" s="22">
         <f>VLOOKUP(U6,Pivot_Tables!D7:E12,2,FALSE)</f>
         <v>26</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K8" s="24">
         <f>VLOOKUP(U6,Pivot_Tables!A19:B24,2,TRUE)</f>
         <v>69061.258064516136</v>
       </c>

</xml_diff>